<commit_message>
Test placement in 7x7cm with updates
</commit_message>
<xml_diff>
--- a/analysis/batteries.xlsx
+++ b/analysis/batteries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konstantinos.kanavou\Documents\git\cmu\chipysat\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DA0D41-FCDE-424B-8A62-4F2AF78AEA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53A5C55-CF9B-4C09-A5EB-A0F3330EE0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{13DE4909-64E5-4074-A7C1-F03D7AF59A6D}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>